<commit_message>
Adding config and mapping xcel sheets
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="12435" windowHeight="4680"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,21 +16,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="10">
   <si>
-    <t>G</t>
+    <t>W</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>air</t>
+  </si>
+  <si>
+    <t>cloud</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>castle</t>
   </si>
   <si>
     <t>T</t>
   </si>
   <si>
-    <t>B</t>
+    <t>launcher</t>
   </si>
   <si>
-    <t>W</t>
+    <t>G</t>
   </si>
   <si>
-    <t>C</t>
+    <t>grass</t>
   </si>
 </sst>
 </file>
@@ -61,19 +76,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,1512 +423,1539 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA19"/>
+  <dimension ref="A1:AD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="3.5703125" style="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="5" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>0</v>
-      </c>
     </row>
-    <row r="2" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA3" s="1">
         <v>2</v>
       </c>
+      <c r="AC3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="1">
         <v>3</v>
       </c>
+      <c r="AC4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="1">
         <v>4</v>
       </c>
+      <c r="AC5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="6" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA7" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z8" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="AA8" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z9" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="AA9" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W10" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W10" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z10" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="AA10" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X11" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="AA11" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z12" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="AA12" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z13" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="AA13" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="AA14" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="AA15" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="AA16" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z17" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="AA17" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA18" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -1992,6 +2034,7 @@
       <c r="Z19" s="1">
         <v>25</v>
       </c>
+      <c r="AA19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added changed configs back
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="10">
   <si>
     <t>W</t>
   </si>
@@ -61,7 +61,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,6 +92,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -105,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -120,6 +126,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -423,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD19"/>
+  <dimension ref="A1:AI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,17 +519,32 @@
       <c r="Z1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA1" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,17 +623,32 @@
       <c r="Z2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AA2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1">
         <v>1</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AH2" t="s">
         <v>1</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AI2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,17 +727,32 @@
       <c r="Z3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="AA3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="1">
         <v>2</v>
       </c>
-      <c r="AC3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD3" t="s">
+      <c r="AH3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,17 +831,32 @@
       <c r="Z4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA4" s="1">
+      <c r="AA4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="1">
         <v>3</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AH4" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AI4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,17 +935,32 @@
       <c r="Z5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA5" s="1">
-        <v>4</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD5" t="s">
+      <c r="AA5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,11 +1039,26 @@
       <c r="Z6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AA6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1038,11 +1137,26 @@
       <c r="Z7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA7" s="1">
+      <c r="AA7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1088,8 +1202,8 @@
       <c r="O8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P8" s="4" t="s">
-        <v>4</v>
+      <c r="P8" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>0</v>
@@ -1121,11 +1235,26 @@
       <c r="Z8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AA8" s="1">
+      <c r="AA8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF8" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1171,8 +1300,8 @@
       <c r="O9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P9" s="4" t="s">
-        <v>4</v>
+      <c r="P9" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>0</v>
@@ -1183,14 +1312,14 @@
       <c r="S9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T9" s="4" t="s">
-        <v>4</v>
+      <c r="T9" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V9" s="4" t="s">
-        <v>4</v>
+      <c r="V9" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>0</v>
@@ -1198,17 +1327,32 @@
       <c r="X9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y9" s="1" t="s">
-        <v>0</v>
+      <c r="Y9" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="Z9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AA9" s="1">
+      <c r="AA9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF9" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1254,8 +1398,8 @@
       <c r="O10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P10" s="4" t="s">
-        <v>4</v>
+      <c r="P10" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>0</v>
@@ -1263,35 +1407,50 @@
       <c r="R10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="S10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="T10" s="4" t="s">
-        <v>4</v>
+      <c r="S10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="W10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>0</v>
+      <c r="V10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AA10" s="1">
+      <c r="AA10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF10" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1337,26 +1496,26 @@
       <c r="O11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P11" s="4" t="s">
-        <v>4</v>
+      <c r="P11" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>4</v>
+      <c r="R11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V11" s="4" t="s">
-        <v>4</v>
+      <c r="V11" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W11" s="4" t="s">
         <v>4</v>
@@ -1364,17 +1523,32 @@
       <c r="X11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Y11" s="1" t="s">
-        <v>0</v>
+      <c r="Y11" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="Z11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AA11" s="1">
+      <c r="AA11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF11" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1420,20 +1594,20 @@
       <c r="O12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="S12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>4</v>
+      <c r="P12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U12" s="4" t="s">
         <v>4</v>
@@ -1453,11 +1627,26 @@
       <c r="Z12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AA12" s="1">
+      <c r="AA12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF12" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1503,20 +1692,20 @@
       <c r="O13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="S13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="T13" s="4" t="s">
-        <v>4</v>
+      <c r="P13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>4</v>
@@ -1536,11 +1725,26 @@
       <c r="Z13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AA13" s="1">
+      <c r="AA13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF13" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1586,20 +1790,20 @@
       <c r="O14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="R14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="S14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="T14" s="4" t="s">
-        <v>4</v>
+      <c r="P14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U14" s="4" t="s">
         <v>4</v>
@@ -1619,343 +1823,418 @@
       <c r="Z14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AA14" s="1">
+      <c r="AA14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF14" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="R15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="S15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="T15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="U15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="V15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="W15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="X15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA15" s="1">
-        <v>14</v>
+      <c r="D17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="W17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF17" s="1">
+        <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="R16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="S16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="T16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="U16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="V16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="W16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="X16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA16" s="1">
-        <v>15</v>
+    <row r="18" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF18" s="1">
+        <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="R17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="S17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="T17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="U17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="V17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="W17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="X17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA17" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="T18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="V18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="W18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA18" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -2034,10 +2313,25 @@
       <c r="Z19" s="1">
         <v>25</v>
       </c>
-      <c r="AA19" s="1"/>
+      <c r="AA19" s="1">
+        <v>26</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>27</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>28</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>29</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>